<commit_message>
Nicer formatting and added missing data
</commit_message>
<xml_diff>
--- a/example_data/With Errors/2024-02-06_SeqLib_SLJS038_MIS2024_BatchF.xlsx
+++ b/example_data/With Errors/2024-02-06_SeqLib_SLJS038_MIS2024_BatchF.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Assay" sheetId="1" state="visible" r:id="rId3"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="428">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="432">
   <si>
     <t xml:space="preserve">NOMADS Library Worksheet</t>
   </si>
@@ -796,6 +796,18 @@
   </si>
   <si>
     <t xml:space="preserve">F2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MIS2345</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MT561</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SWJS044_F2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PCTB150_F2</t>
   </si>
   <si>
     <t xml:space="preserve">14</t>
@@ -2799,7 +2811,7 @@
   </sheetPr>
   <dimension ref="A1:L70"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -3871,7 +3883,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="9" id="{4766FF80-B551-4EF3-8ED1-94B64D51AB42}">
+          <x14:cfRule type="expression" priority="9" id="{E28E4E19-577F-4A3F-9E10-BDE86557A02F}">
             <xm:f>COUNTIF($C$66,reference!$E$4)</xm:f>
             <x14:dxf>
               <fill>
@@ -3897,8 +3909,8 @@
   </sheetPr>
   <dimension ref="A1:M111"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I16" activeCellId="0" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.01953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4564,30 +4576,42 @@
       <c r="B16" s="74" t="s">
         <v>181</v>
       </c>
-      <c r="C16" s="75"/>
-      <c r="D16" s="89"/>
-      <c r="E16" s="90"/>
-      <c r="F16" s="90"/>
-      <c r="G16" s="84"/>
-      <c r="H16" s="78"/>
-      <c r="I16" s="79" t="str">
+      <c r="C16" s="75" t="s">
+        <v>182</v>
+      </c>
+      <c r="D16" s="89" t="s">
+        <v>183</v>
+      </c>
+      <c r="E16" s="76" t="s">
+        <v>184</v>
+      </c>
+      <c r="F16" s="83" t="s">
+        <v>185</v>
+      </c>
+      <c r="G16" s="84" t="n">
+        <v>10</v>
+      </c>
+      <c r="H16" s="78" t="n">
+        <v>1</v>
+      </c>
+      <c r="I16" s="79" t="n">
         <f aca="false">IF(OR(tbl_SeqLib[[#This Row],[Qubit PCR '[DNA'] (ng/µl)]]="", tbl_SeqLib[[#This Row],[PCR Dilution Factor]]=""),"",SUM(tbl_SeqLib[[#This Row],[Qubit PCR '[DNA'] (ng/µl)]]*tbl_SeqLib[[#This Row],[PCR Dilution Factor]]))</f>
-        <v/>
+        <v>10</v>
       </c>
       <c r="J16" s="85" t="s">
-        <v>182</v>
-      </c>
-      <c r="K16" s="86" t="str">
+        <v>186</v>
+      </c>
+      <c r="K16" s="86" t="n">
         <f aca="false">IFERROR(IF(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]=0,endrepair_maxvol,IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]))),"")</f>
-        <v/>
-      </c>
-      <c r="L16" s="86" t="str">
+        <v>10</v>
+      </c>
+      <c r="L16" s="86" t="n">
         <f aca="false">IFERROR(SUM(endrepair_maxvol-K16),"")</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="M16" s="79" t="str">
         <f aca="false">IF(ISBLANK(tbl_SeqLib[[#This Row],[sWGA Identifier]]),"",_xlfn.CONCAT(exp_id,"_",tbl_SeqLib[[#This Row],[Well]]))</f>
-        <v/>
+        <v>SLJS038_F2</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4595,7 +4619,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="74" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="C17" s="75"/>
       <c r="D17" s="89"/>
@@ -4608,7 +4632,7 @@
         <v/>
       </c>
       <c r="J17" s="85" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="K17" s="86" t="str">
         <f aca="false">IFERROR(IF(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]=0,endrepair_maxvol,IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]))),"")</f>
@@ -4628,7 +4652,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="74" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="C18" s="75"/>
       <c r="D18" s="89"/>
@@ -4641,7 +4665,7 @@
         <v/>
       </c>
       <c r="J18" s="85" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="K18" s="86" t="str">
         <f aca="false">IFERROR(IF(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]=0,endrepair_maxvol,IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]))),"")</f>
@@ -4661,7 +4685,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="74" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="C19" s="75"/>
       <c r="D19" s="89"/>
@@ -4674,7 +4698,7 @@
         <v/>
       </c>
       <c r="J19" s="85" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="K19" s="86" t="str">
         <f aca="false">IFERROR(IF(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]=0,endrepair_maxvol,IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]))),"")</f>
@@ -4694,7 +4718,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="74" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="C20" s="75"/>
       <c r="D20" s="89"/>
@@ -4707,7 +4731,7 @@
         <v/>
       </c>
       <c r="J20" s="85" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="K20" s="86" t="str">
         <f aca="false">IFERROR(IF(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]=0,endrepair_maxvol,IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]))),"")</f>
@@ -4727,7 +4751,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="74" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="C21" s="75"/>
       <c r="D21" s="89"/>
@@ -4740,7 +4764,7 @@
         <v/>
       </c>
       <c r="J21" s="85" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="K21" s="86" t="str">
         <f aca="false">IFERROR(IF(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]=0,endrepair_maxvol,IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]))),"")</f>
@@ -4760,7 +4784,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="73" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="C22" s="75"/>
       <c r="D22" s="89"/>
@@ -4773,7 +4797,7 @@
         <v/>
       </c>
       <c r="J22" s="85" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="K22" s="86" t="str">
         <f aca="false">IFERROR(IF(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]=0,endrepair_maxvol,IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]))),"")</f>
@@ -4793,7 +4817,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="73" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="C23" s="91"/>
       <c r="D23" s="92"/>
@@ -4806,7 +4830,7 @@
         <v/>
       </c>
       <c r="J23" s="85" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="K23" s="86" t="str">
         <f aca="false">IFERROR(IF(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]=0,endrepair_maxvol,IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]))),"")</f>
@@ -4826,7 +4850,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="73" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="C24" s="91"/>
       <c r="D24" s="92"/>
@@ -4839,7 +4863,7 @@
         <v/>
       </c>
       <c r="J24" s="85" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="K24" s="86" t="str">
         <f aca="false">IFERROR(IF(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]=0,endrepair_maxvol,IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]))),"")</f>
@@ -4859,7 +4883,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="73" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="C25" s="91"/>
       <c r="D25" s="92"/>
@@ -4872,7 +4896,7 @@
         <v/>
       </c>
       <c r="J25" s="85" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="K25" s="86" t="str">
         <f aca="false">IFERROR(IF(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]=0,endrepair_maxvol,IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]))),"")</f>
@@ -4892,7 +4916,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="73" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="C26" s="91"/>
       <c r="D26" s="92"/>
@@ -4905,7 +4929,7 @@
         <v/>
       </c>
       <c r="J26" s="85" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="K26" s="86" t="str">
         <f aca="false">IFERROR(IF(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]=0,endrepair_maxvol,IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]))),"")</f>
@@ -4925,7 +4949,7 @@
         <v>25</v>
       </c>
       <c r="B27" s="73" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="C27" s="91"/>
       <c r="D27" s="92"/>
@@ -4938,7 +4962,7 @@
         <v/>
       </c>
       <c r="J27" s="85" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="K27" s="86" t="str">
         <f aca="false">IFERROR(IF(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]=0,endrepair_maxvol,IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]))),"")</f>
@@ -4958,7 +4982,7 @@
         <v>26</v>
       </c>
       <c r="B28" s="73" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="C28" s="91"/>
       <c r="D28" s="92"/>
@@ -4971,7 +4995,7 @@
         <v/>
       </c>
       <c r="J28" s="85" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="K28" s="86" t="str">
         <f aca="false">IFERROR(IF(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]=0,endrepair_maxvol,IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]))),"")</f>
@@ -4991,7 +5015,7 @@
         <v>27</v>
       </c>
       <c r="B29" s="73" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="C29" s="91"/>
       <c r="D29" s="92"/>
@@ -5004,7 +5028,7 @@
         <v/>
       </c>
       <c r="J29" s="85" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="K29" s="86" t="str">
         <f aca="false">IFERROR(IF(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]=0,endrepair_maxvol,IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]))),"")</f>
@@ -5024,7 +5048,7 @@
         <v>28</v>
       </c>
       <c r="B30" s="73" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="C30" s="91"/>
       <c r="D30" s="92"/>
@@ -5037,7 +5061,7 @@
         <v/>
       </c>
       <c r="J30" s="85" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="K30" s="86" t="str">
         <f aca="false">IFERROR(IF(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]=0,endrepair_maxvol,IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]))),"")</f>
@@ -5057,7 +5081,7 @@
         <v>29</v>
       </c>
       <c r="B31" s="73" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="C31" s="91"/>
       <c r="D31" s="92"/>
@@ -5070,7 +5094,7 @@
         <v/>
       </c>
       <c r="J31" s="85" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="K31" s="86" t="str">
         <f aca="false">IFERROR(IF(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]=0,endrepair_maxvol,IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]))),"")</f>
@@ -5090,7 +5114,7 @@
         <v>30</v>
       </c>
       <c r="B32" s="73" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="C32" s="91"/>
       <c r="D32" s="92"/>
@@ -5103,7 +5127,7 @@
         <v/>
       </c>
       <c r="J32" s="85" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="K32" s="86" t="str">
         <f aca="false">IFERROR(IF(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]=0,endrepair_maxvol,IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]))),"")</f>
@@ -5123,7 +5147,7 @@
         <v>31</v>
       </c>
       <c r="B33" s="73" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="C33" s="91"/>
       <c r="D33" s="92"/>
@@ -5136,7 +5160,7 @@
         <v/>
       </c>
       <c r="J33" s="85" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="K33" s="86" t="str">
         <f aca="false">IFERROR(IF(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]=0,endrepair_maxvol,IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]))),"")</f>
@@ -5156,7 +5180,7 @@
         <v>32</v>
       </c>
       <c r="B34" s="73" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="C34" s="91"/>
       <c r="D34" s="92"/>
@@ -5169,7 +5193,7 @@
         <v/>
       </c>
       <c r="J34" s="85" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="K34" s="86" t="str">
         <f aca="false">IFERROR(IF(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]=0,endrepair_maxvol,IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]))),"")</f>
@@ -5189,7 +5213,7 @@
         <v>33</v>
       </c>
       <c r="B35" s="73" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="C35" s="91"/>
       <c r="D35" s="92"/>
@@ -5202,7 +5226,7 @@
         <v/>
       </c>
       <c r="J35" s="85" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="K35" s="86" t="str">
         <f aca="false">IFERROR(IF(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]=0,endrepair_maxvol,IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]))),"")</f>
@@ -5222,7 +5246,7 @@
         <v>34</v>
       </c>
       <c r="B36" s="73" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="C36" s="91"/>
       <c r="D36" s="92"/>
@@ -5235,7 +5259,7 @@
         <v/>
       </c>
       <c r="J36" s="85" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="K36" s="86" t="str">
         <f aca="false">IFERROR(IF(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]=0,endrepair_maxvol,IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]))),"")</f>
@@ -5255,7 +5279,7 @@
         <v>35</v>
       </c>
       <c r="B37" s="73" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="C37" s="91"/>
       <c r="D37" s="92"/>
@@ -5268,7 +5292,7 @@
         <v/>
       </c>
       <c r="J37" s="85" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="K37" s="86" t="str">
         <f aca="false">IFERROR(IF(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]=0,endrepair_maxvol,IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]))),"")</f>
@@ -5288,7 +5312,7 @@
         <v>36</v>
       </c>
       <c r="B38" s="73" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="C38" s="91"/>
       <c r="D38" s="92"/>
@@ -5301,7 +5325,7 @@
         <v/>
       </c>
       <c r="J38" s="85" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="K38" s="86" t="str">
         <f aca="false">IFERROR(IF(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]=0,endrepair_maxvol,IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]))),"")</f>
@@ -5321,7 +5345,7 @@
         <v>37</v>
       </c>
       <c r="B39" s="73" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="C39" s="91"/>
       <c r="D39" s="92"/>
@@ -5334,7 +5358,7 @@
         <v/>
       </c>
       <c r="J39" s="85" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="K39" s="86" t="str">
         <f aca="false">IFERROR(IF(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]=0,endrepair_maxvol,IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]))),"")</f>
@@ -5354,7 +5378,7 @@
         <v>38</v>
       </c>
       <c r="B40" s="73" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="C40" s="91"/>
       <c r="D40" s="92"/>
@@ -5367,7 +5391,7 @@
         <v/>
       </c>
       <c r="J40" s="85" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="K40" s="86" t="str">
         <f aca="false">IFERROR(IF(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]=0,endrepair_maxvol,IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]))),"")</f>
@@ -5387,7 +5411,7 @@
         <v>39</v>
       </c>
       <c r="B41" s="73" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="C41" s="91"/>
       <c r="D41" s="92"/>
@@ -5400,7 +5424,7 @@
         <v/>
       </c>
       <c r="J41" s="85" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="K41" s="86" t="str">
         <f aca="false">IFERROR(IF(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]=0,endrepair_maxvol,IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]))),"")</f>
@@ -5420,7 +5444,7 @@
         <v>40</v>
       </c>
       <c r="B42" s="73" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="C42" s="91"/>
       <c r="D42" s="92"/>
@@ -5433,7 +5457,7 @@
         <v/>
       </c>
       <c r="J42" s="85" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="K42" s="86" t="str">
         <f aca="false">IFERROR(IF(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]=0,endrepair_maxvol,IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]))),"")</f>
@@ -5453,7 +5477,7 @@
         <v>41</v>
       </c>
       <c r="B43" s="73" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="C43" s="91"/>
       <c r="D43" s="92"/>
@@ -5466,7 +5490,7 @@
         <v/>
       </c>
       <c r="J43" s="85" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="K43" s="86" t="str">
         <f aca="false">IFERROR(IF(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]=0,endrepair_maxvol,IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]))),"")</f>
@@ -5486,7 +5510,7 @@
         <v>42</v>
       </c>
       <c r="B44" s="73" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="C44" s="91"/>
       <c r="D44" s="92"/>
@@ -5499,7 +5523,7 @@
         <v/>
       </c>
       <c r="J44" s="85" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="K44" s="86" t="str">
         <f aca="false">IFERROR(IF(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]=0,endrepair_maxvol,IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]))),"")</f>
@@ -5519,7 +5543,7 @@
         <v>43</v>
       </c>
       <c r="B45" s="73" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="C45" s="91"/>
       <c r="D45" s="92"/>
@@ -5532,7 +5556,7 @@
         <v/>
       </c>
       <c r="J45" s="85" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="K45" s="86" t="str">
         <f aca="false">IFERROR(IF(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]=0,endrepair_maxvol,IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]))),"")</f>
@@ -5552,7 +5576,7 @@
         <v>44</v>
       </c>
       <c r="B46" s="73" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="C46" s="91"/>
       <c r="D46" s="92"/>
@@ -5565,7 +5589,7 @@
         <v/>
       </c>
       <c r="J46" s="85" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="K46" s="86" t="str">
         <f aca="false">IFERROR(IF(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]=0,endrepair_maxvol,IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]))),"")</f>
@@ -5585,7 +5609,7 @@
         <v>45</v>
       </c>
       <c r="B47" s="73" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="C47" s="91"/>
       <c r="D47" s="92"/>
@@ -5598,7 +5622,7 @@
         <v/>
       </c>
       <c r="J47" s="85" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="K47" s="86" t="str">
         <f aca="false">IFERROR(IF(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]=0,endrepair_maxvol,IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]))),"")</f>
@@ -5618,7 +5642,7 @@
         <v>46</v>
       </c>
       <c r="B48" s="73" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="C48" s="91"/>
       <c r="D48" s="92"/>
@@ -5631,7 +5655,7 @@
         <v/>
       </c>
       <c r="J48" s="85" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="K48" s="86" t="str">
         <f aca="false">IFERROR(IF(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]=0,endrepair_maxvol,IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]))),"")</f>
@@ -5651,7 +5675,7 @@
         <v>47</v>
       </c>
       <c r="B49" s="73" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="C49" s="91"/>
       <c r="D49" s="92"/>
@@ -5664,7 +5688,7 @@
         <v/>
       </c>
       <c r="J49" s="85" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="K49" s="86" t="str">
         <f aca="false">IFERROR(IF(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]=0,endrepair_maxvol,IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]))),"")</f>
@@ -5684,7 +5708,7 @@
         <v>48</v>
       </c>
       <c r="B50" s="73" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="C50" s="91"/>
       <c r="D50" s="92"/>
@@ -5697,7 +5721,7 @@
         <v/>
       </c>
       <c r="J50" s="85" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="K50" s="86" t="str">
         <f aca="false">IFERROR(IF(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]=0,endrepair_maxvol,IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]))),"")</f>
@@ -5717,7 +5741,7 @@
         <v>49</v>
       </c>
       <c r="B51" s="73" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="C51" s="91"/>
       <c r="D51" s="92"/>
@@ -5730,7 +5754,7 @@
         <v/>
       </c>
       <c r="J51" s="85" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="K51" s="86" t="str">
         <f aca="false">IFERROR(IF(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]=0,endrepair_maxvol,IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]))),"")</f>
@@ -5750,7 +5774,7 @@
         <v>50</v>
       </c>
       <c r="B52" s="73" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="C52" s="91"/>
       <c r="D52" s="92"/>
@@ -5763,7 +5787,7 @@
         <v/>
       </c>
       <c r="J52" s="85" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="K52" s="86" t="str">
         <f aca="false">IFERROR(IF(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]=0,endrepair_maxvol,IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]))),"")</f>
@@ -5783,7 +5807,7 @@
         <v>51</v>
       </c>
       <c r="B53" s="73" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="C53" s="91"/>
       <c r="D53" s="92"/>
@@ -5796,7 +5820,7 @@
         <v/>
       </c>
       <c r="J53" s="85" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="K53" s="86" t="str">
         <f aca="false">IFERROR(IF(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]=0,endrepair_maxvol,IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]))),"")</f>
@@ -5816,7 +5840,7 @@
         <v>52</v>
       </c>
       <c r="B54" s="73" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="C54" s="91"/>
       <c r="D54" s="92"/>
@@ -5829,7 +5853,7 @@
         <v/>
       </c>
       <c r="J54" s="85" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="K54" s="86" t="str">
         <f aca="false">IFERROR(IF(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]=0,endrepair_maxvol,IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]))),"")</f>
@@ -5849,7 +5873,7 @@
         <v>53</v>
       </c>
       <c r="B55" s="73" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="C55" s="91"/>
       <c r="D55" s="92"/>
@@ -5862,7 +5886,7 @@
         <v/>
       </c>
       <c r="J55" s="85" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="K55" s="86" t="str">
         <f aca="false">IFERROR(IF(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]=0,endrepair_maxvol,IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]))),"")</f>
@@ -5882,7 +5906,7 @@
         <v>54</v>
       </c>
       <c r="B56" s="73" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="C56" s="91"/>
       <c r="D56" s="92"/>
@@ -5895,7 +5919,7 @@
         <v/>
       </c>
       <c r="J56" s="85" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="K56" s="86" t="str">
         <f aca="false">IFERROR(IF(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]=0,endrepair_maxvol,IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]))),"")</f>
@@ -5915,7 +5939,7 @@
         <v>55</v>
       </c>
       <c r="B57" s="73" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="C57" s="91"/>
       <c r="D57" s="92"/>
@@ -5928,7 +5952,7 @@
         <v/>
       </c>
       <c r="J57" s="85" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="K57" s="86" t="str">
         <f aca="false">IFERROR(IF(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]=0,endrepair_maxvol,IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]))),"")</f>
@@ -5948,7 +5972,7 @@
         <v>56</v>
       </c>
       <c r="B58" s="73" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="C58" s="91"/>
       <c r="D58" s="92"/>
@@ -5961,7 +5985,7 @@
         <v/>
       </c>
       <c r="J58" s="85" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="K58" s="86" t="str">
         <f aca="false">IFERROR(IF(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]=0,endrepair_maxvol,IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]))),"")</f>
@@ -5981,7 +6005,7 @@
         <v>57</v>
       </c>
       <c r="B59" s="73" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="C59" s="91"/>
       <c r="D59" s="92"/>
@@ -5994,7 +6018,7 @@
         <v/>
       </c>
       <c r="J59" s="85" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="K59" s="86" t="str">
         <f aca="false">IFERROR(IF(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]=0,endrepair_maxvol,IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]))),"")</f>
@@ -6014,7 +6038,7 @@
         <v>58</v>
       </c>
       <c r="B60" s="73" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="C60" s="91"/>
       <c r="D60" s="92"/>
@@ -6027,7 +6051,7 @@
         <v/>
       </c>
       <c r="J60" s="85" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="K60" s="86" t="str">
         <f aca="false">IFERROR(IF(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]=0,endrepair_maxvol,IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]))),"")</f>
@@ -6047,7 +6071,7 @@
         <v>59</v>
       </c>
       <c r="B61" s="73" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="C61" s="91"/>
       <c r="D61" s="92"/>
@@ -6060,7 +6084,7 @@
         <v/>
       </c>
       <c r="J61" s="85" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="K61" s="86" t="str">
         <f aca="false">IFERROR(IF(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]=0,endrepair_maxvol,IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]))),"")</f>
@@ -6080,7 +6104,7 @@
         <v>60</v>
       </c>
       <c r="B62" s="73" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="C62" s="91"/>
       <c r="D62" s="92"/>
@@ -6093,7 +6117,7 @@
         <v/>
       </c>
       <c r="J62" s="85" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="K62" s="86" t="str">
         <f aca="false">IFERROR(IF(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]=0,endrepair_maxvol,IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]))),"")</f>
@@ -6113,7 +6137,7 @@
         <v>61</v>
       </c>
       <c r="B63" s="73" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="C63" s="91"/>
       <c r="D63" s="92"/>
@@ -6126,7 +6150,7 @@
         <v/>
       </c>
       <c r="J63" s="85" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="K63" s="86" t="str">
         <f aca="false">IFERROR(IF(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]=0,endrepair_maxvol,IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]))),"")</f>
@@ -6146,7 +6170,7 @@
         <v>62</v>
       </c>
       <c r="B64" s="73" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="C64" s="91"/>
       <c r="D64" s="92"/>
@@ -6159,7 +6183,7 @@
         <v/>
       </c>
       <c r="J64" s="85" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="K64" s="86" t="str">
         <f aca="false">IFERROR(IF(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]=0,endrepair_maxvol,IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]))),"")</f>
@@ -6179,7 +6203,7 @@
         <v>63</v>
       </c>
       <c r="B65" s="73" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="C65" s="91"/>
       <c r="D65" s="92"/>
@@ -6192,7 +6216,7 @@
         <v/>
       </c>
       <c r="J65" s="85" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="K65" s="86" t="str">
         <f aca="false">IFERROR(IF(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]=0,endrepair_maxvol,IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]))),"")</f>
@@ -6212,7 +6236,7 @@
         <v>64</v>
       </c>
       <c r="B66" s="73" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="C66" s="91"/>
       <c r="D66" s="92"/>
@@ -6225,7 +6249,7 @@
         <v/>
       </c>
       <c r="J66" s="85" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="K66" s="86" t="str">
         <f aca="false">IFERROR(IF(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]=0,endrepair_maxvol,IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]))),"")</f>
@@ -6245,7 +6269,7 @@
         <v>65</v>
       </c>
       <c r="B67" s="73" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="C67" s="91"/>
       <c r="D67" s="92"/>
@@ -6258,7 +6282,7 @@
         <v/>
       </c>
       <c r="J67" s="85" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="K67" s="86" t="str">
         <f aca="false">IFERROR(IF(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]=0,endrepair_maxvol,IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]))),"")</f>
@@ -6278,7 +6302,7 @@
         <v>66</v>
       </c>
       <c r="B68" s="73" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="C68" s="91"/>
       <c r="D68" s="92"/>
@@ -6291,7 +6315,7 @@
         <v/>
       </c>
       <c r="J68" s="85" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="K68" s="86" t="str">
         <f aca="false">IFERROR(IF(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]=0,endrepair_maxvol,IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]))),"")</f>
@@ -6311,7 +6335,7 @@
         <v>67</v>
       </c>
       <c r="B69" s="73" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="C69" s="91"/>
       <c r="D69" s="92"/>
@@ -6324,7 +6348,7 @@
         <v/>
       </c>
       <c r="J69" s="85" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="K69" s="86" t="str">
         <f aca="false">IFERROR(IF(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]=0,endrepair_maxvol,IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]))),"")</f>
@@ -6344,7 +6368,7 @@
         <v>68</v>
       </c>
       <c r="B70" s="73" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="C70" s="91"/>
       <c r="D70" s="92"/>
@@ -6357,7 +6381,7 @@
         <v/>
       </c>
       <c r="J70" s="85" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="K70" s="86" t="str">
         <f aca="false">IFERROR(IF(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]=0,endrepair_maxvol,IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]))),"")</f>
@@ -6377,7 +6401,7 @@
         <v>69</v>
       </c>
       <c r="B71" s="73" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="C71" s="91"/>
       <c r="D71" s="92"/>
@@ -6390,7 +6414,7 @@
         <v/>
       </c>
       <c r="J71" s="85" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="K71" s="86" t="str">
         <f aca="false">IFERROR(IF(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]=0,endrepair_maxvol,IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]))),"")</f>
@@ -6410,7 +6434,7 @@
         <v>70</v>
       </c>
       <c r="B72" s="73" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="C72" s="91"/>
       <c r="D72" s="92"/>
@@ -6423,7 +6447,7 @@
         <v/>
       </c>
       <c r="J72" s="85" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="K72" s="86" t="str">
         <f aca="false">IFERROR(IF(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]=0,endrepair_maxvol,IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]))),"")</f>
@@ -6443,7 +6467,7 @@
         <v>71</v>
       </c>
       <c r="B73" s="73" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="C73" s="91"/>
       <c r="D73" s="92"/>
@@ -6456,7 +6480,7 @@
         <v/>
       </c>
       <c r="J73" s="85" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="K73" s="86" t="str">
         <f aca="false">IFERROR(IF(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]=0,endrepair_maxvol,IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]))),"")</f>
@@ -6476,7 +6500,7 @@
         <v>72</v>
       </c>
       <c r="B74" s="73" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="C74" s="91"/>
       <c r="D74" s="92"/>
@@ -6489,7 +6513,7 @@
         <v/>
       </c>
       <c r="J74" s="85" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
       <c r="K74" s="86" t="str">
         <f aca="false">IFERROR(IF(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]=0,endrepair_maxvol,IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]))),"")</f>
@@ -6509,7 +6533,7 @@
         <v>73</v>
       </c>
       <c r="B75" s="73" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="C75" s="91"/>
       <c r="D75" s="92"/>
@@ -6522,7 +6546,7 @@
         <v/>
       </c>
       <c r="J75" s="85" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="K75" s="86" t="str">
         <f aca="false">IFERROR(IF(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]=0,endrepair_maxvol,IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]))),"")</f>
@@ -6542,7 +6566,7 @@
         <v>74</v>
       </c>
       <c r="B76" s="73" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="C76" s="91"/>
       <c r="D76" s="92"/>
@@ -6555,7 +6579,7 @@
         <v/>
       </c>
       <c r="J76" s="85" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="K76" s="86" t="str">
         <f aca="false">IFERROR(IF(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]=0,endrepair_maxvol,IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]))),"")</f>
@@ -6575,7 +6599,7 @@
         <v>75</v>
       </c>
       <c r="B77" s="73" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="C77" s="91"/>
       <c r="D77" s="92"/>
@@ -6588,7 +6612,7 @@
         <v/>
       </c>
       <c r="J77" s="85" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
       <c r="K77" s="86" t="str">
         <f aca="false">IFERROR(IF(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]=0,endrepair_maxvol,IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]))),"")</f>
@@ -6608,7 +6632,7 @@
         <v>76</v>
       </c>
       <c r="B78" s="73" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="C78" s="91"/>
       <c r="D78" s="92"/>
@@ -6621,7 +6645,7 @@
         <v/>
       </c>
       <c r="J78" s="85" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
       <c r="K78" s="86" t="str">
         <f aca="false">IFERROR(IF(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]=0,endrepair_maxvol,IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]))),"")</f>
@@ -6641,7 +6665,7 @@
         <v>77</v>
       </c>
       <c r="B79" s="73" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="C79" s="91"/>
       <c r="D79" s="92"/>
@@ -6654,7 +6678,7 @@
         <v/>
       </c>
       <c r="J79" s="85" t="s">
-        <v>308</v>
+        <v>312</v>
       </c>
       <c r="K79" s="86" t="str">
         <f aca="false">IFERROR(IF(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]=0,endrepair_maxvol,IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]))),"")</f>
@@ -6674,7 +6698,7 @@
         <v>78</v>
       </c>
       <c r="B80" s="73" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="C80" s="91"/>
       <c r="D80" s="92"/>
@@ -6687,7 +6711,7 @@
         <v/>
       </c>
       <c r="J80" s="85" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="K80" s="86" t="str">
         <f aca="false">IFERROR(IF(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]=0,endrepair_maxvol,IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]))),"")</f>
@@ -6707,7 +6731,7 @@
         <v>79</v>
       </c>
       <c r="B81" s="73" t="s">
-        <v>311</v>
+        <v>315</v>
       </c>
       <c r="C81" s="91"/>
       <c r="D81" s="92"/>
@@ -6720,7 +6744,7 @@
         <v/>
       </c>
       <c r="J81" s="85" t="s">
-        <v>312</v>
+        <v>316</v>
       </c>
       <c r="K81" s="86" t="str">
         <f aca="false">IFERROR(IF(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]=0,endrepair_maxvol,IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]))),"")</f>
@@ -6740,7 +6764,7 @@
         <v>80</v>
       </c>
       <c r="B82" s="73" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="C82" s="91"/>
       <c r="D82" s="92"/>
@@ -6753,7 +6777,7 @@
         <v/>
       </c>
       <c r="J82" s="85" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="K82" s="86" t="str">
         <f aca="false">IFERROR(IF(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]=0,endrepair_maxvol,IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]))),"")</f>
@@ -6773,7 +6797,7 @@
         <v>81</v>
       </c>
       <c r="B83" s="73" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
       <c r="C83" s="91"/>
       <c r="D83" s="92"/>
@@ -6786,7 +6810,7 @@
         <v/>
       </c>
       <c r="J83" s="85" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="K83" s="86" t="str">
         <f aca="false">IFERROR(IF(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]=0,endrepair_maxvol,IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]))),"")</f>
@@ -6806,7 +6830,7 @@
         <v>82</v>
       </c>
       <c r="B84" s="73" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="C84" s="91"/>
       <c r="D84" s="92"/>
@@ -6819,7 +6843,7 @@
         <v/>
       </c>
       <c r="J84" s="85" t="s">
-        <v>318</v>
+        <v>322</v>
       </c>
       <c r="K84" s="86" t="str">
         <f aca="false">IFERROR(IF(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]=0,endrepair_maxvol,IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]))),"")</f>
@@ -6839,7 +6863,7 @@
         <v>83</v>
       </c>
       <c r="B85" s="73" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="C85" s="91"/>
       <c r="D85" s="92"/>
@@ -6852,7 +6876,7 @@
         <v/>
       </c>
       <c r="J85" s="85" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="K85" s="86" t="str">
         <f aca="false">IFERROR(IF(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]=0,endrepair_maxvol,IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]))),"")</f>
@@ -6872,7 +6896,7 @@
         <v>84</v>
       </c>
       <c r="B86" s="73" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="C86" s="91"/>
       <c r="D86" s="92"/>
@@ -6885,7 +6909,7 @@
         <v/>
       </c>
       <c r="J86" s="85" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="K86" s="86" t="str">
         <f aca="false">IFERROR(IF(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]=0,endrepair_maxvol,IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]))),"")</f>
@@ -6905,7 +6929,7 @@
         <v>85</v>
       </c>
       <c r="B87" s="73" t="s">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="C87" s="91"/>
       <c r="D87" s="92"/>
@@ -6918,7 +6942,7 @@
         <v/>
       </c>
       <c r="J87" s="85" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="K87" s="86" t="str">
         <f aca="false">IFERROR(IF(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]=0,endrepair_maxvol,IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]))),"")</f>
@@ -6938,7 +6962,7 @@
         <v>86</v>
       </c>
       <c r="B88" s="73" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="C88" s="91"/>
       <c r="D88" s="92"/>
@@ -6951,7 +6975,7 @@
         <v/>
       </c>
       <c r="J88" s="85" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
       <c r="K88" s="86" t="str">
         <f aca="false">IFERROR(IF(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]=0,endrepair_maxvol,IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]))),"")</f>
@@ -6971,7 +6995,7 @@
         <v>87</v>
       </c>
       <c r="B89" s="73" t="s">
-        <v>327</v>
+        <v>331</v>
       </c>
       <c r="C89" s="91"/>
       <c r="D89" s="92"/>
@@ -6984,7 +7008,7 @@
         <v/>
       </c>
       <c r="J89" s="85" t="s">
-        <v>328</v>
+        <v>332</v>
       </c>
       <c r="K89" s="86" t="str">
         <f aca="false">IFERROR(IF(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]=0,endrepair_maxvol,IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]))),"")</f>
@@ -7004,7 +7028,7 @@
         <v>88</v>
       </c>
       <c r="B90" s="73" t="s">
-        <v>329</v>
+        <v>333</v>
       </c>
       <c r="C90" s="91"/>
       <c r="D90" s="92"/>
@@ -7017,7 +7041,7 @@
         <v/>
       </c>
       <c r="J90" s="85" t="s">
-        <v>330</v>
+        <v>334</v>
       </c>
       <c r="K90" s="86" t="str">
         <f aca="false">IFERROR(IF(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]=0,endrepair_maxvol,IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]))),"")</f>
@@ -7037,7 +7061,7 @@
         <v>89</v>
       </c>
       <c r="B91" s="73" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="C91" s="91"/>
       <c r="D91" s="92"/>
@@ -7050,7 +7074,7 @@
         <v/>
       </c>
       <c r="J91" s="85" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c r="K91" s="86" t="str">
         <f aca="false">IFERROR(IF(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]=0,endrepair_maxvol,IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]))),"")</f>
@@ -7070,7 +7094,7 @@
         <v>90</v>
       </c>
       <c r="B92" s="73" t="s">
-        <v>333</v>
+        <v>337</v>
       </c>
       <c r="C92" s="91"/>
       <c r="D92" s="92"/>
@@ -7083,7 +7107,7 @@
         <v/>
       </c>
       <c r="J92" s="85" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="K92" s="86" t="str">
         <f aca="false">IFERROR(IF(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]=0,endrepair_maxvol,IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]))),"")</f>
@@ -7103,7 +7127,7 @@
         <v>91</v>
       </c>
       <c r="B93" s="73" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="C93" s="91"/>
       <c r="D93" s="92"/>
@@ -7116,7 +7140,7 @@
         <v/>
       </c>
       <c r="J93" s="85" t="s">
-        <v>336</v>
+        <v>340</v>
       </c>
       <c r="K93" s="86" t="str">
         <f aca="false">IFERROR(IF(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]=0,endrepair_maxvol,IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]))),"")</f>
@@ -7136,7 +7160,7 @@
         <v>92</v>
       </c>
       <c r="B94" s="73" t="s">
-        <v>337</v>
+        <v>341</v>
       </c>
       <c r="C94" s="91"/>
       <c r="D94" s="92"/>
@@ -7149,7 +7173,7 @@
         <v/>
       </c>
       <c r="J94" s="85" t="s">
-        <v>338</v>
+        <v>342</v>
       </c>
       <c r="K94" s="86" t="str">
         <f aca="false">IFERROR(IF(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]=0,endrepair_maxvol,IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]))),"")</f>
@@ -7169,7 +7193,7 @@
         <v>93</v>
       </c>
       <c r="B95" s="73" t="s">
-        <v>339</v>
+        <v>343</v>
       </c>
       <c r="C95" s="91"/>
       <c r="D95" s="92"/>
@@ -7182,7 +7206,7 @@
         <v/>
       </c>
       <c r="J95" s="85" t="s">
-        <v>340</v>
+        <v>344</v>
       </c>
       <c r="K95" s="86" t="str">
         <f aca="false">IFERROR(IF(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]=0,endrepair_maxvol,IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]))),"")</f>
@@ -7202,7 +7226,7 @@
         <v>94</v>
       </c>
       <c r="B96" s="73" t="s">
-        <v>341</v>
+        <v>345</v>
       </c>
       <c r="C96" s="91"/>
       <c r="D96" s="92"/>
@@ -7215,7 +7239,7 @@
         <v/>
       </c>
       <c r="J96" s="85" t="s">
-        <v>342</v>
+        <v>346</v>
       </c>
       <c r="K96" s="86" t="str">
         <f aca="false">IFERROR(IF(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]=0,endrepair_maxvol,IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]))),"")</f>
@@ -7235,7 +7259,7 @@
         <v>95</v>
       </c>
       <c r="B97" s="73" t="s">
-        <v>343</v>
+        <v>347</v>
       </c>
       <c r="C97" s="91"/>
       <c r="D97" s="92"/>
@@ -7248,7 +7272,7 @@
         <v/>
       </c>
       <c r="J97" s="85" t="s">
-        <v>344</v>
+        <v>348</v>
       </c>
       <c r="K97" s="86" t="str">
         <f aca="false">IFERROR(IF(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]=0,endrepair_maxvol,IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]))),"")</f>
@@ -7268,7 +7292,7 @@
         <v>96</v>
       </c>
       <c r="B98" s="93" t="s">
-        <v>345</v>
+        <v>349</v>
       </c>
       <c r="C98" s="91"/>
       <c r="D98" s="92"/>
@@ -7281,7 +7305,7 @@
         <v/>
       </c>
       <c r="J98" s="95" t="s">
-        <v>346</v>
+        <v>350</v>
       </c>
       <c r="K98" s="96" t="str">
         <f aca="false">IFERROR(IF(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]=0,endrepair_maxvol,IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]))),"")</f>
@@ -7409,7 +7433,7 @@
       <formula>COUNTIF(C3,"")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C13:D22 E16:F22">
+  <conditionalFormatting sqref="C13:D22 E17:F22">
     <cfRule type="expression" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="21">
       <formula>COUNTIF(C13,"")</formula>
     </cfRule>
@@ -7458,77 +7482,77 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="100" t="s">
-        <v>347</v>
+        <v>351</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="101" t="s">
-        <v>348</v>
+        <v>352</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="102" t="s">
-        <v>349</v>
+        <v>353</v>
       </c>
       <c r="B3" s="101" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="102" t="s">
-        <v>351</v>
+        <v>355</v>
       </c>
       <c r="B4" s="101" t="s">
-        <v>352</v>
+        <v>356</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="14" t="s">
-        <v>353</v>
+        <v>357</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="103" t="s">
-        <v>354</v>
+        <v>358</v>
       </c>
       <c r="B7" s="101" t="s">
-        <v>355</v>
+        <v>359</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="103" t="s">
-        <v>356</v>
+        <v>360</v>
       </c>
       <c r="B8" s="101" t="s">
-        <v>357</v>
+        <v>361</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="103" t="s">
-        <v>358</v>
+        <v>362</v>
       </c>
       <c r="B9" s="101" t="s">
-        <v>359</v>
+        <v>363</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="101" t="s">
-        <v>360</v>
+        <v>364</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="104" t="s">
-        <v>361</v>
+        <v>365</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="62" t="s">
-        <v>362</v>
+        <v>366</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="62" t="s">
-        <v>363</v>
+        <v>367</v>
       </c>
     </row>
   </sheetData>
@@ -7569,99 +7593,99 @@
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="105" t="s">
-        <v>364</v>
+        <v>368</v>
       </c>
       <c r="C1" s="106"/>
       <c r="D1" s="106"/>
       <c r="E1" s="105" t="s">
-        <v>365</v>
+        <v>369</v>
       </c>
       <c r="G1" s="105" t="s">
-        <v>366</v>
+        <v>370</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="107" t="s">
-        <v>367</v>
+        <v>371</v>
       </c>
       <c r="B2" s="108"/>
       <c r="C2" s="108"/>
       <c r="E2" s="108" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
       <c r="G2" s="109" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="H2" s="109" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="J2" s="109" t="s">
-        <v>371</v>
+        <v>375</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="45" t="s">
-        <v>372</v>
+        <v>376</v>
       </c>
       <c r="B3" s="62" t="n">
         <v>500</v>
       </c>
       <c r="C3" s="62" t="s">
-        <v>373</v>
+        <v>377</v>
       </c>
       <c r="E3" s="62" t="s">
-        <v>374</v>
+        <v>378</v>
       </c>
       <c r="G3" s="110" t="s">
         <v>6</v>
       </c>
       <c r="H3" s="110" t="s">
-        <v>375</v>
+        <v>379</v>
       </c>
       <c r="J3" s="110" t="s">
-        <v>376</v>
+        <v>380</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="45" t="s">
-        <v>377</v>
+        <v>381</v>
       </c>
       <c r="B4" s="62" t="n">
         <v>10</v>
       </c>
       <c r="C4" s="62" t="s">
-        <v>378</v>
+        <v>382</v>
       </c>
       <c r="D4" s="111"/>
       <c r="E4" s="62" t="s">
-        <v>379</v>
+        <v>383</v>
       </c>
       <c r="G4" s="110" t="s">
-        <v>380</v>
+        <v>384</v>
       </c>
       <c r="H4" s="110" t="s">
-        <v>381</v>
+        <v>385</v>
       </c>
       <c r="J4" s="110" t="s">
-        <v>382</v>
+        <v>386</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="45" t="s">
-        <v>383</v>
+        <v>387</v>
       </c>
       <c r="B5" s="62" t="n">
         <v>800</v>
       </c>
       <c r="C5" s="62" t="s">
-        <v>373</v>
+        <v>377</v>
       </c>
       <c r="D5" s="111"/>
       <c r="G5" s="110" t="s">
-        <v>384</v>
+        <v>388</v>
       </c>
       <c r="H5" s="110" t="s">
-        <v>385</v>
+        <v>389</v>
       </c>
       <c r="J5" s="110" t="s">
         <v>18</v>
@@ -7669,81 +7693,81 @@
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="45" t="s">
-        <v>386</v>
+        <v>390</v>
       </c>
       <c r="B6" s="62" t="n">
         <v>65</v>
       </c>
       <c r="C6" s="62" t="s">
-        <v>378</v>
+        <v>382</v>
       </c>
       <c r="E6" s="108" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
       <c r="G6" s="112" t="s">
-        <v>387</v>
+        <v>391</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="45" t="s">
-        <v>388</v>
+        <v>392</v>
       </c>
       <c r="B7" s="62" t="n">
         <v>400</v>
       </c>
       <c r="C7" s="62" t="s">
-        <v>373</v>
+        <v>377</v>
       </c>
       <c r="E7" s="62" t="s">
-        <v>374</v>
+        <v>378</v>
       </c>
       <c r="G7" s="112" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="45" t="s">
-        <v>390</v>
+        <v>394</v>
       </c>
       <c r="B8" s="62" t="n">
         <v>12</v>
       </c>
       <c r="C8" s="62" t="s">
-        <v>378</v>
+        <v>382</v>
       </c>
       <c r="E8" s="62" t="s">
-        <v>379</v>
+        <v>383</v>
       </c>
       <c r="G8" s="113" t="s">
-        <v>391</v>
+        <v>395</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G9" s="112" t="s">
-        <v>392</v>
+        <v>396</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="107" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="B10" s="108"/>
       <c r="C10" s="108"/>
       <c r="G10" s="112" t="s">
-        <v>394</v>
+        <v>398</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="45" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
       <c r="B11" s="62" t="s">
-        <v>396</v>
+        <v>400</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="45" t="s">
-        <v>397</v>
+        <v>401</v>
       </c>
       <c r="B12" s="62" t="n">
         <v>3</v>
@@ -7800,73 +7824,73 @@
   <sheetData>
     <row r="1" s="45" customFormat="true" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="45" t="s">
-        <v>398</v>
+        <v>402</v>
       </c>
       <c r="B1" s="45" t="s">
-        <v>399</v>
+        <v>403</v>
       </c>
       <c r="C1" s="45" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
       <c r="D1" s="45" t="s">
-        <v>401</v>
+        <v>405</v>
       </c>
       <c r="E1" s="45" t="s">
-        <v>402</v>
+        <v>406</v>
       </c>
       <c r="F1" s="45" t="s">
-        <v>403</v>
+        <v>407</v>
       </c>
       <c r="G1" s="45" t="s">
-        <v>404</v>
+        <v>408</v>
       </c>
       <c r="H1" s="45" t="s">
-        <v>405</v>
+        <v>409</v>
       </c>
       <c r="I1" s="45" t="s">
-        <v>406</v>
+        <v>410</v>
       </c>
       <c r="J1" s="45" t="s">
-        <v>407</v>
+        <v>411</v>
       </c>
       <c r="K1" s="45" t="s">
-        <v>408</v>
+        <v>412</v>
       </c>
       <c r="L1" s="45" t="s">
-        <v>409</v>
+        <v>413</v>
       </c>
       <c r="M1" s="45" t="s">
-        <v>410</v>
+        <v>414</v>
       </c>
       <c r="N1" s="45" t="s">
-        <v>411</v>
+        <v>415</v>
       </c>
       <c r="O1" s="45" t="s">
-        <v>412</v>
+        <v>416</v>
       </c>
       <c r="P1" s="45" t="s">
-        <v>413</v>
+        <v>417</v>
       </c>
       <c r="Q1" s="45" t="s">
-        <v>414</v>
+        <v>418</v>
       </c>
       <c r="R1" s="45" t="s">
-        <v>415</v>
+        <v>419</v>
       </c>
       <c r="S1" s="45" t="s">
-        <v>416</v>
+        <v>420</v>
       </c>
       <c r="T1" s="45" t="s">
-        <v>417</v>
+        <v>421</v>
       </c>
       <c r="U1" s="45" t="s">
-        <v>418</v>
+        <v>422</v>
       </c>
       <c r="V1" s="45" t="s">
-        <v>419</v>
+        <v>423</v>
       </c>
       <c r="W1" s="45" t="s">
-        <v>420</v>
+        <v>424</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8001,28 +8025,28 @@
   <sheetData>
     <row r="1" customFormat="false" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="115" t="s">
-        <v>421</v>
+        <v>425</v>
       </c>
       <c r="B1" s="115" t="s">
-        <v>422</v>
+        <v>426</v>
       </c>
       <c r="C1" s="115" t="s">
-        <v>398</v>
+        <v>402</v>
       </c>
       <c r="D1" s="115" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
       <c r="E1" s="115" t="s">
-        <v>424</v>
+        <v>428</v>
       </c>
       <c r="F1" s="115" t="s">
-        <v>425</v>
+        <v>429</v>
       </c>
       <c r="G1" s="115" t="s">
-        <v>426</v>
+        <v>430</v>
       </c>
       <c r="H1" s="115" t="s">
-        <v>427</v>
+        <v>431</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8470,35 +8494,35 @@
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="62" t="str">
         <f aca="false">IF(LEN(Library!C16)=0,"",Library!C16)</f>
-        <v/>
+        <v>MIS2345</v>
       </c>
       <c r="B15" s="62" t="str">
         <f aca="false">IF(LEN(Library!D16)=0,"",Library!D16)</f>
-        <v/>
+        <v>MT561</v>
       </c>
       <c r="C15" s="62" t="str">
         <f aca="false">IF(LEN(Library!E16)=0,"",exp_id)</f>
-        <v/>
+        <v>SLJS038</v>
       </c>
       <c r="D15" s="62" t="str">
         <f aca="false">IF(LEN(Library!E16)=0,"",Library!E16)</f>
-        <v/>
+        <v>SWJS044_F2</v>
       </c>
       <c r="E15" s="62" t="str">
         <f aca="false">IF(LEN(Library!F16)=0,"",Library!F16)</f>
-        <v/>
+        <v>PCTB150_F2</v>
       </c>
       <c r="F15" s="62" t="str">
         <f aca="false">IF(LEN(Library!M16)=0,"",Library!M16)</f>
-        <v/>
+        <v>SLJS038_F2</v>
       </c>
       <c r="G15" s="62" t="str">
         <f aca="false">IF(LEN(Library!E16)=0,"",_xlfn.CONCAT("barcode",Library!J16))</f>
-        <v/>
-      </c>
-      <c r="H15" s="62" t="str">
+        <v>barcode14</v>
+      </c>
+      <c r="H15" s="62" t="n">
         <f aca="false">IF(LEN(Library!K16)=0,"",Library!K16)</f>
-        <v/>
+        <v>10</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>